<commit_message>
Add advanced NLP features New Advanced NLP Module: - Named Entity Recognition (NER)   - Extract people, organizations, locations   - Count and rank entity mentions   - Support for 8 entity types
- Keyword Extraction
  - RAKE algorithm (phrase-based)
  - TF-IDF (statistical)
  - Customizable top-N keywords

- Topic Detection
  - Automatic topic categorization
  - Themes: quality, price, service, features, experience
  - Keyword clustering

- Text Complexity Analysis
  - Flesch Reading Ease score
  - Flesch-Kincaid Grade Level
  - Readability interpretation
  - Avg words per sentence

Integration:
- Added to unified pipeline
- Method chaining support
- CLI arguments for each feature
- Enhanced reporting

Dependencies:
- spaCy for NER
- RAKE-NLTK for keywords
- sklearn for TF-IDF
- Custom readability calculator
</commit_message>
<xml_diff>
--- a/output/results.xlsx
+++ b/output/results.xlsx
@@ -502,35 +502,35 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="D2" t="n">
-        <v>361.54</v>
+        <v>351.54</v>
       </c>
       <c r="E2" t="n">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Decent product for the price. Had some minor issues.</t>
+          <t>Average product. Works as described but nothing impressive.</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H2" t="n">
-        <v>0.05833333333333333</v>
+        <v>0.425</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4333333333333333</v>
+        <v>0.7</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -545,27 +545,27 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="D3" t="n">
-        <v>417.9</v>
+        <v>407.9</v>
       </c>
       <c r="E3" t="n">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Works fine. Installation was a bit tricky.</t>
+          <t>Meets basic expectations. Could be better.</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.25</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5</v>
+        <v>0.3125</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -573,7 +573,7 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -598,21 +598,21 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Good but could be better. Missing some features.</t>
+          <t>Decent for the price. Not great, not terrible.</t>
         </is>
       </c>
       <c r="G4" t="n">
         <v>8</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.08888888888888886</v>
       </c>
       <c r="I4" t="n">
-        <v>0.3833333333333334</v>
+        <v>0.8055555555555555</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -631,27 +631,27 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>243.66</v>
+        <v>303.66</v>
       </c>
       <c r="E5" t="n">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Not worth it.</t>
+          <t>Broke after two days. Very disappointed with the quality.</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.15</v>
+        <v>-0.9750000000000001</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
@@ -674,27 +674,27 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>3.1</v>
       </c>
       <c r="D6" t="n">
-        <v>507.22</v>
+        <v>317.22</v>
       </c>
       <c r="E6" t="n">
-        <v>239</v>
+        <v>144</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Best purchase I've made this year. The build quality is exceptional, features are exactly what I needed, and customer service was fantastic. Worth every penny. Will definitely buy from this brand again.</t>
+          <t>Best purchase I've made this year. Works perfectly and looks amazing.</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="H6" t="n">
-        <v>0.4361111111111111</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="I6" t="n">
-        <v>0.5083333333333334</v>
+        <v>0.7333333333333334</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
@@ -717,27 +717,27 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4.9</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>469.67</v>
+        <v>279.67</v>
       </c>
       <c r="E7" t="n">
-        <v>202</v>
+        <v>107</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Best purchase I've made this year. The build quality is exceptional, features are exactly what I needed, and customer service was fantastic. Worth every penny. Will definitely buy from this brand again.</t>
+          <t>Best purchase I've made this year. Works perfectly and looks amazing.</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="H7" t="n">
-        <v>0.4361111111111111</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="I7" t="n">
-        <v>0.5083333333333334</v>
+        <v>0.7333333333333334</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -745,7 +745,7 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
@@ -760,27 +760,27 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4.3</v>
+        <v>2.4</v>
       </c>
       <c r="D8" t="n">
-        <v>628.7</v>
+        <v>438.7</v>
       </c>
       <c r="E8" t="n">
-        <v>214</v>
+        <v>119</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Exceeded expectations in every way. I did extensive research before buying and this was the best choice. The quality, functionality, and value are all exceptional. Already recommended to three friends.</t>
+          <t>Absolutely perfect. Been using it daily and it's still like new.</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H8" t="n">
-        <v>0.5555555555555555</v>
+        <v>0.3787878787878787</v>
       </c>
       <c r="I8" t="n">
-        <v>0.5444444444444444</v>
+        <v>0.4848484848484849</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -788,7 +788,7 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
@@ -803,35 +803,35 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.4</v>
+        <v>2.9</v>
       </c>
       <c r="D9" t="n">
-        <v>174.9</v>
+        <v>224.9</v>
       </c>
       <c r="E9" t="n">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Poor quality.</t>
+          <t>Cheap materials, poor design. Regret buying this.</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.4</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.6</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -846,35 +846,35 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="D10" t="n">
-        <v>351.94</v>
+        <v>341.94</v>
       </c>
       <c r="E10" t="n">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Decent product for the price. Had some minor issues.</t>
+          <t>Average product. Works as described but nothing impressive.</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10" t="n">
-        <v>0.05833333333333333</v>
+        <v>0.425</v>
       </c>
       <c r="I10" t="n">
-        <v>0.4333333333333333</v>
+        <v>0.7</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -889,27 +889,27 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>4.4</v>
+        <v>2.5</v>
       </c>
       <c r="D11" t="n">
-        <v>436.64</v>
+        <v>246.64</v>
       </c>
       <c r="E11" t="n">
-        <v>219</v>
+        <v>124</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Best purchase I've made this year. The build quality is exceptional, features are exactly what I needed, and customer service was fantastic. Worth every penny. Will definitely buy from this brand again.</t>
+          <t>Best purchase I've made this year. Works perfectly and looks amazing.</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4361111111111111</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="I11" t="n">
-        <v>0.5083333333333334</v>
+        <v>0.7333333333333334</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
@@ -932,27 +932,27 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>4.4</v>
+        <v>2.4</v>
       </c>
       <c r="D12" t="n">
-        <v>449.09</v>
+        <v>249.09</v>
       </c>
       <c r="E12" t="n">
-        <v>211</v>
+        <v>111</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Five stars all the way! This has made my life so much easier. The design is intuitive, setup was straightforward, and performance is top-notch. Can't imagine going back to my old setup now.</t>
+          <t>Incredible! Fast shipping, great packaging, and the product is fantastic.</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="H12" t="n">
-        <v>0.335</v>
+        <v>0.6</v>
       </c>
       <c r="I12" t="n">
-        <v>0.355</v>
+        <v>0.7875</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
@@ -985,17 +985,17 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>It's okay but nothing special. Works as expected.</t>
+          <t>It's okay. Nothing special but does the job.</t>
         </is>
       </c>
       <c r="G13" t="n">
         <v>8</v>
       </c>
       <c r="H13" t="n">
-        <v>0.2523809523809524</v>
+        <v>0.4285714285714286</v>
       </c>
       <c r="I13" t="n">
-        <v>0.4904761904761905</v>
+        <v>0.5357142857142857</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1018,27 +1018,27 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>4.9</v>
+        <v>3</v>
       </c>
       <c r="D14" t="n">
-        <v>660.09</v>
+        <v>470.09</v>
       </c>
       <c r="E14" t="n">
-        <v>258</v>
+        <v>163</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Exceeded expectations in every way. I did extensive research before buying and this was the best choice. The quality, functionality, and value are all exceptional. Already recommended to three friends.</t>
+          <t>Absolutely perfect. Been using it daily and it's still like new.</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H14" t="n">
-        <v>0.5555555555555555</v>
+        <v>0.3787878787878787</v>
       </c>
       <c r="I14" t="n">
-        <v>0.5444444444444444</v>
+        <v>0.4848484848484849</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1046,7 +1046,7 @@
         </is>
       </c>
       <c r="K14" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
@@ -1061,27 +1061,27 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4.9</v>
+        <v>3</v>
       </c>
       <c r="D15" t="n">
-        <v>439.09</v>
+        <v>249.09</v>
       </c>
       <c r="E15" t="n">
-        <v>213</v>
+        <v>118</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Exceeded expectations in every way. I did extensive research before buying and this was the best choice. The quality, functionality, and value are all exceptional. Already recommended to three friends.</t>
+          <t>Absolutely perfect. Been using it daily and it's still like new.</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H15" t="n">
-        <v>0.5555555555555555</v>
+        <v>0.3787878787878787</v>
       </c>
       <c r="I15" t="n">
-        <v>0.5444444444444444</v>
+        <v>0.4848484848484849</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1089,7 +1089,7 @@
         </is>
       </c>
       <c r="K15" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16">
@@ -1104,27 +1104,27 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3.5</v>
+        <v>4.1</v>
       </c>
       <c r="D16" t="n">
-        <v>507.1</v>
+        <v>567.1</v>
       </c>
       <c r="E16" t="n">
-        <v>176</v>
+        <v>205</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Not worth it.</t>
+          <t>Broke after two days. Very disappointed with the quality.</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.15</v>
+        <v>-0.9750000000000001</v>
       </c>
       <c r="I16" t="n">
-        <v>0.1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="K16" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
@@ -1147,27 +1147,27 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D17" t="n">
-        <v>582.41</v>
+        <v>382.41</v>
       </c>
       <c r="E17" t="n">
-        <v>242</v>
+        <v>142</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Incredible product! I was skeptical at first but after using it daily for several weeks, I'm completely sold. The attention to detail is remarkable and it just works flawlessly. My colleagues are asking where I got it.</t>
+          <t>Outstanding product! Exceeded all my expectations. Five stars!</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="H17" t="n">
-        <v>0.325</v>
+        <v>0.78125</v>
       </c>
       <c r="I17" t="n">
-        <v>0.4854166666666667</v>
+        <v>0.875</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1175,7 +1175,7 @@
         </is>
       </c>
       <c r="K17" t="n">
-        <v>37</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
@@ -1190,27 +1190,27 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2.4</v>
+        <v>2.9</v>
       </c>
       <c r="D18" t="n">
-        <v>262.47</v>
+        <v>312.47</v>
       </c>
       <c r="E18" t="n">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Terrible product. Don't buy.</t>
+          <t>Terrible product. Complete waste of money. Don't buy this!</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H18" t="n">
-        <v>-1</v>
+        <v>-0.3833333333333333</v>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0.4666666666666666</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1218,7 +1218,7 @@
         </is>
       </c>
       <c r="K18" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19">
@@ -1233,27 +1233,27 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4.6</v>
+        <v>2.7</v>
       </c>
       <c r="D19" t="n">
-        <v>568.21</v>
+        <v>378.21</v>
       </c>
       <c r="E19" t="n">
-        <v>246</v>
+        <v>152</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Exceeded expectations in every way. I did extensive research before buying and this was the best choice. The quality, functionality, and value are all exceptional. Already recommended to three friends.</t>
+          <t>Absolutely perfect. Been using it daily and it's still like new.</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H19" t="n">
-        <v>0.5555555555555555</v>
+        <v>0.3787878787878787</v>
       </c>
       <c r="I19" t="n">
-        <v>0.5444444444444444</v>
+        <v>0.4848484848484849</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1261,7 +1261,7 @@
         </is>
       </c>
       <c r="K19" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20">
@@ -1276,35 +1276,35 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2.6</v>
+        <v>3</v>
       </c>
       <c r="D20" t="n">
-        <v>440.37</v>
+        <v>480.37</v>
       </c>
       <c r="E20" t="n">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Broke after one week.</t>
+          <t>Not worth it at all. Save your money.</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>-0.15</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="K20" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
@@ -1319,27 +1319,27 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="D21" t="n">
-        <v>583.13</v>
+        <v>423.13</v>
       </c>
       <c r="E21" t="n">
-        <v>269</v>
+        <v>189</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Best purchase I've made this year. The build quality is exceptional, features are exactly what I needed, and customer service was fantastic. Worth every penny. Will definitely buy from this brand again.</t>
+          <t>Best purchase I've made this year. Works perfectly and looks amazing.</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="H21" t="n">
-        <v>0.4361111111111111</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="I21" t="n">
-        <v>0.5083333333333334</v>
+        <v>0.7333333333333334</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1347,7 +1347,7 @@
         </is>
       </c>
       <c r="K21" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22">
@@ -1362,27 +1362,27 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="D22" t="n">
-        <v>193.03</v>
+        <v>253.03</v>
       </c>
       <c r="E22" t="n">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Not worth it.</t>
+          <t>Broke after two days. Very disappointed with the quality.</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.15</v>
+        <v>-0.9750000000000001</v>
       </c>
       <c r="I22" t="n">
-        <v>0.1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1390,7 +1390,7 @@
         </is>
       </c>
       <c r="K22" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23">
@@ -1405,27 +1405,27 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>5</v>
+        <v>3.7</v>
       </c>
       <c r="D23" t="n">
-        <v>633.48</v>
+        <v>503.48</v>
       </c>
       <c r="E23" t="n">
-        <v>255</v>
+        <v>190</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Best purchase I've made this year. The build quality is exceptional, features are exactly what I needed, and customer service was fantastic. Worth every penny. Will definitely buy from this brand again.</t>
+          <t>Best purchase I've made this year. Works perfectly and looks amazing.</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="H23" t="n">
-        <v>0.4361111111111111</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="I23" t="n">
-        <v>0.5083333333333334</v>
+        <v>0.7333333333333334</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1433,7 +1433,7 @@
         </is>
       </c>
       <c r="K23" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24">
@@ -1448,27 +1448,27 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2.6</v>
+        <v>3.1</v>
       </c>
       <c r="D24" t="n">
-        <v>301.89</v>
+        <v>351.89</v>
       </c>
       <c r="E24" t="n">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Terrible product. Don't buy.</t>
+          <t>Terrible product. Complete waste of money. Don't buy this!</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H24" t="n">
-        <v>-1</v>
+        <v>-0.3833333333333333</v>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0.4666666666666666</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1476,7 +1476,7 @@
         </is>
       </c>
       <c r="K24" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25">
@@ -1491,35 +1491,35 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D25" t="n">
-        <v>376.42</v>
+        <v>366.42</v>
       </c>
       <c r="E25" t="n">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Decent product for the price. Had some minor issues.</t>
+          <t>Average product. Works as described but nothing impressive.</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H25" t="n">
-        <v>0.05833333333333333</v>
+        <v>0.425</v>
       </c>
       <c r="I25" t="n">
-        <v>0.4333333333333333</v>
+        <v>0.7</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="K25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26">
@@ -1544,17 +1544,17 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Average quality. Not bad but not great either.</t>
+          <t>It works. That's about all I can say.</t>
         </is>
       </c>
       <c r="G26" t="n">
         <v>8</v>
       </c>
       <c r="H26" t="n">
-        <v>-0.06666666666666669</v>
+        <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>0.6055555555555555</v>
+        <v>0</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1577,35 +1577,35 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>2.8</v>
+        <v>2.7</v>
       </c>
       <c r="D27" t="n">
-        <v>593.35</v>
+        <v>583.35</v>
       </c>
       <c r="E27" t="n">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Decent product for the price. Had some minor issues.</t>
+          <t>Average product. Works as described but nothing impressive.</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H27" t="n">
-        <v>0.05833333333333333</v>
+        <v>0.425</v>
       </c>
       <c r="I27" t="n">
-        <v>0.4333333333333333</v>
+        <v>0.7</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="K27" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
@@ -1620,27 +1620,27 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2.1</v>
+        <v>2.7</v>
       </c>
       <c r="D28" t="n">
-        <v>295.71</v>
+        <v>355.71</v>
       </c>
       <c r="E28" t="n">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Very disappointed.</t>
+          <t>Worst purchase ever. Customer service was unhelpful too.</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="I28" t="n">
-        <v>0.9750000000000001</v>
+        <v>1</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1648,7 +1648,7 @@
         </is>
       </c>
       <c r="K28" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29">
@@ -1663,27 +1663,27 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1.9</v>
+        <v>2.5</v>
       </c>
       <c r="D29" t="n">
-        <v>253.58</v>
+        <v>313.58</v>
       </c>
       <c r="E29" t="n">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Very disappointed.</t>
+          <t>Worst purchase ever. Customer service was unhelpful too.</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H29" t="n">
-        <v>-0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="I29" t="n">
-        <v>0.9750000000000001</v>
+        <v>1</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -1691,7 +1691,7 @@
         </is>
       </c>
       <c r="K29" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30">
@@ -1706,35 +1706,35 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="D30" t="n">
-        <v>435.82</v>
+        <v>475.82</v>
       </c>
       <c r="E30" t="n">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Broke after one week.</t>
+          <t>Not worth it at all. Save your money.</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>-0.15</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="K30" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
@@ -1749,27 +1749,27 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>5</v>
+        <v>3.3</v>
       </c>
       <c r="D31" t="n">
-        <v>646.26</v>
+        <v>476.26</v>
       </c>
       <c r="E31" t="n">
-        <v>245</v>
+        <v>160</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Best purchase I've made this year. The build quality is exceptional, features are exactly what I needed, and customer service was fantastic. Worth every penny. Will definitely buy from this brand again.</t>
+          <t>Best purchase I've made this year. Works perfectly and looks amazing.</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="H31" t="n">
-        <v>0.4361111111111111</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="I31" t="n">
-        <v>0.5083333333333334</v>
+        <v>0.7333333333333334</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -1777,7 +1777,7 @@
         </is>
       </c>
       <c r="K31" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32">
@@ -1792,27 +1792,27 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="D32" t="n">
-        <v>213.84</v>
+        <v>203.84</v>
       </c>
       <c r="E32" t="n">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Works fine. Installation was a bit tricky.</t>
+          <t>Meets basic expectations. Could be better.</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H32" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.25</v>
       </c>
       <c r="I32" t="n">
-        <v>0.5</v>
+        <v>0.3125</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -1820,7 +1820,7 @@
         </is>
       </c>
       <c r="K32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33">
@@ -1835,27 +1835,27 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>5</v>
+        <v>3.3</v>
       </c>
       <c r="D33" t="n">
-        <v>677.37</v>
+        <v>507.37</v>
       </c>
       <c r="E33" t="n">
-        <v>244</v>
+        <v>159</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Absolutely love this product! The quality is outstanding and it exceeded all my expectations. Been using it for months now with zero issues. Highly recommend to anyone looking for reliability and performance.</t>
+          <t>Love it! Excellent quality and great value for money. Highly recommend!</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="H33" t="n">
-        <v>0.4283333333333333</v>
+        <v>0.65625</v>
       </c>
       <c r="I33" t="n">
-        <v>0.6716666666666667</v>
+        <v>0.7225</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -1863,7 +1863,7 @@
         </is>
       </c>
       <c r="K33" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34">
@@ -1888,17 +1888,17 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Average quality. Not bad but not great either.</t>
+          <t>It works. That's about all I can say.</t>
         </is>
       </c>
       <c r="G34" t="n">
         <v>8</v>
       </c>
       <c r="H34" t="n">
-        <v>-0.06666666666666669</v>
+        <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>0.6055555555555555</v>
+        <v>0</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -1921,27 +1921,27 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>3.9</v>
+        <v>4.4</v>
       </c>
       <c r="D35" t="n">
-        <v>405.73</v>
+        <v>455.73</v>
       </c>
       <c r="E35" t="n">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Terrible product. Don't buy.</t>
+          <t>Terrible product. Complete waste of money. Don't buy this!</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H35" t="n">
-        <v>-1</v>
+        <v>-0.3833333333333333</v>
       </c>
       <c r="I35" t="n">
-        <v>1</v>
+        <v>0.4666666666666666</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -1949,7 +1949,7 @@
         </is>
       </c>
       <c r="K35" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36">
@@ -1964,27 +1964,27 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>4.8</v>
+        <v>2.9</v>
       </c>
       <c r="D36" t="n">
-        <v>473.02</v>
+        <v>283.02</v>
       </c>
       <c r="E36" t="n">
-        <v>198</v>
+        <v>103</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Exceeded expectations in every way. I did extensive research before buying and this was the best choice. The quality, functionality, and value are all exceptional. Already recommended to three friends.</t>
+          <t>Absolutely perfect. Been using it daily and it's still like new.</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H36" t="n">
-        <v>0.5555555555555555</v>
+        <v>0.3787878787878787</v>
       </c>
       <c r="I36" t="n">
-        <v>0.5444444444444444</v>
+        <v>0.4848484848484849</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -1992,7 +1992,7 @@
         </is>
       </c>
       <c r="K36" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37">
@@ -2007,27 +2007,27 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>5</v>
+        <v>3.6</v>
       </c>
       <c r="D37" t="n">
-        <v>548.14</v>
+        <v>408.14</v>
       </c>
       <c r="E37" t="n">
-        <v>216</v>
+        <v>146</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Five stars all the way! This has made my life so much easier. The design is intuitive, setup was straightforward, and performance is top-notch. Can't imagine going back to my old setup now.</t>
+          <t>Incredible! Fast shipping, great packaging, and the product is fantastic.</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="H37" t="n">
-        <v>0.335</v>
+        <v>0.6</v>
       </c>
       <c r="I37" t="n">
-        <v>0.355</v>
+        <v>0.7875</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -2035,7 +2035,7 @@
         </is>
       </c>
       <c r="K37" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38">
@@ -2050,27 +2050,27 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2.2</v>
+        <v>2.7</v>
       </c>
       <c r="D38" t="n">
-        <v>261.58</v>
+        <v>311.58</v>
       </c>
       <c r="E38" t="n">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Terrible product. Don't buy.</t>
+          <t>Terrible product. Complete waste of money. Don't buy this!</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H38" t="n">
-        <v>-1</v>
+        <v>-0.3833333333333333</v>
       </c>
       <c r="I38" t="n">
-        <v>1</v>
+        <v>0.4666666666666666</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -2078,7 +2078,7 @@
         </is>
       </c>
       <c r="K38" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39">
@@ -2093,27 +2093,27 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>4.3</v>
+        <v>2.3</v>
       </c>
       <c r="D39" t="n">
-        <v>476.53</v>
+        <v>276.53</v>
       </c>
       <c r="E39" t="n">
-        <v>191</v>
+        <v>90</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Five stars all the way! This has made my life so much easier. The design is intuitive, setup was straightforward, and performance is top-notch. Can't imagine going back to my old setup now.</t>
+          <t>Incredible! Fast shipping, great packaging, and the product is fantastic.</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="H39" t="n">
-        <v>0.335</v>
+        <v>0.6</v>
       </c>
       <c r="I39" t="n">
-        <v>0.355</v>
+        <v>0.7875</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -2121,7 +2121,7 @@
         </is>
       </c>
       <c r="K39" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40">
@@ -2146,17 +2146,17 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>It's okay but nothing special. Works as expected.</t>
+          <t>It's okay. Nothing special but does the job.</t>
         </is>
       </c>
       <c r="G40" t="n">
         <v>8</v>
       </c>
       <c r="H40" t="n">
-        <v>0.2523809523809524</v>
+        <v>0.4285714285714286</v>
       </c>
       <c r="I40" t="n">
-        <v>0.4904761904761905</v>
+        <v>0.5357142857142857</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -2179,27 +2179,27 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="D41" t="n">
-        <v>536.27</v>
+        <v>386.27</v>
       </c>
       <c r="E41" t="n">
-        <v>278</v>
+        <v>203</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Exceeded expectations in every way. I did extensive research before buying and this was the best choice. The quality, functionality, and value are all exceptional. Already recommended to three friends.</t>
+          <t>Absolutely perfect. Been using it daily and it's still like new.</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H41" t="n">
-        <v>0.5555555555555555</v>
+        <v>0.3787878787878787</v>
       </c>
       <c r="I41" t="n">
-        <v>0.5444444444444444</v>
+        <v>0.4848484848484849</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -2207,7 +2207,7 @@
         </is>
       </c>
       <c r="K41" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42">
@@ -2222,27 +2222,27 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2.6</v>
+        <v>3.2</v>
       </c>
       <c r="D42" t="n">
-        <v>529.05</v>
+        <v>589.05</v>
       </c>
       <c r="E42" t="n">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Not worth it.</t>
+          <t>Broke after two days. Very disappointed with the quality.</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H42" t="n">
-        <v>-0.15</v>
+        <v>-0.9750000000000001</v>
       </c>
       <c r="I42" t="n">
-        <v>0.1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -2250,7 +2250,7 @@
         </is>
       </c>
       <c r="K42" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43">
@@ -2265,27 +2265,27 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>4.7</v>
+        <v>2.5</v>
       </c>
       <c r="D43" t="n">
-        <v>478.35</v>
+        <v>258.35</v>
       </c>
       <c r="E43" t="n">
-        <v>252</v>
+        <v>142</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Incredible product! I was skeptical at first but after using it daily for several weeks, I'm completely sold. The attention to detail is remarkable and it just works flawlessly. My colleagues are asking where I got it.</t>
+          <t>Outstanding product! Exceeded all my expectations. Five stars!</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="H43" t="n">
-        <v>0.325</v>
+        <v>0.78125</v>
       </c>
       <c r="I43" t="n">
-        <v>0.4854166666666667</v>
+        <v>0.875</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -2293,7 +2293,7 @@
         </is>
       </c>
       <c r="K43" t="n">
-        <v>37</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44">
@@ -2308,27 +2308,27 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="D44" t="n">
-        <v>233.45</v>
+        <v>293.45</v>
       </c>
       <c r="E44" t="n">
-        <v>122</v>
+        <v>152</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Very disappointed.</t>
+          <t>Worst purchase ever. Customer service was unhelpful too.</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H44" t="n">
-        <v>-0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="I44" t="n">
-        <v>0.9750000000000001</v>
+        <v>1</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -2336,7 +2336,7 @@
         </is>
       </c>
       <c r="K44" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45">
@@ -2351,27 +2351,27 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1.6</v>
+        <v>2.2</v>
       </c>
       <c r="D45" t="n">
-        <v>195.65</v>
+        <v>255.65</v>
       </c>
       <c r="E45" t="n">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Very disappointed.</t>
+          <t>Worst purchase ever. Customer service was unhelpful too.</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H45" t="n">
-        <v>-0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="I45" t="n">
-        <v>0.9750000000000001</v>
+        <v>1</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -2379,7 +2379,7 @@
         </is>
       </c>
       <c r="K45" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46">
@@ -2394,35 +2394,35 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="D46" t="n">
-        <v>267.79</v>
+        <v>257.79</v>
       </c>
       <c r="E46" t="n">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Decent product for the price. Had some minor issues.</t>
+          <t>Average product. Works as described but nothing impressive.</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H46" t="n">
-        <v>0.05833333333333333</v>
+        <v>0.425</v>
       </c>
       <c r="I46" t="n">
-        <v>0.4333333333333333</v>
+        <v>0.7</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="K46" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47">
@@ -2437,27 +2437,27 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="D47" t="n">
-        <v>261.3</v>
+        <v>251.3</v>
       </c>
       <c r="E47" t="n">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Works fine. Installation was a bit tricky.</t>
+          <t>Meets basic expectations. Could be better.</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H47" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.25</v>
       </c>
       <c r="I47" t="n">
-        <v>0.5</v>
+        <v>0.3125</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -2465,7 +2465,7 @@
         </is>
       </c>
       <c r="K47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48">
@@ -2480,27 +2480,27 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>2.2</v>
+        <v>2.7</v>
       </c>
       <c r="D48" t="n">
-        <v>249.41</v>
+        <v>299.41</v>
       </c>
       <c r="E48" t="n">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Terrible product. Don't buy.</t>
+          <t>Terrible product. Complete waste of money. Don't buy this!</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H48" t="n">
-        <v>-1</v>
+        <v>-0.3833333333333333</v>
       </c>
       <c r="I48" t="n">
-        <v>1</v>
+        <v>0.4666666666666666</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -2508,7 +2508,7 @@
         </is>
       </c>
       <c r="K48" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49">
@@ -2523,35 +2523,35 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="D49" t="n">
-        <v>431.62</v>
+        <v>471.62</v>
       </c>
       <c r="E49" t="n">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Broke after one week.</t>
+          <t>Not worth it at all. Save your money.</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H49" t="n">
-        <v>0</v>
+        <v>-0.15</v>
       </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="K49" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50">
@@ -2566,27 +2566,27 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>2.3</v>
+        <v>2.9</v>
       </c>
       <c r="D50" t="n">
-        <v>314.64</v>
+        <v>374.64</v>
       </c>
       <c r="E50" t="n">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Very disappointed.</t>
+          <t>Worst purchase ever. Customer service was unhelpful too.</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H50" t="n">
-        <v>-0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="I50" t="n">
-        <v>0.9750000000000001</v>
+        <v>1</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -2594,7 +2594,7 @@
         </is>
       </c>
       <c r="K50" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51">
@@ -2619,21 +2619,21 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Good but could be better. Missing some features.</t>
+          <t>Decent for the price. Not great, not terrible.</t>
         </is>
       </c>
       <c r="G51" t="n">
         <v>8</v>
       </c>
       <c r="H51" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.08888888888888886</v>
       </c>
       <c r="I51" t="n">
-        <v>0.3833333333333334</v>
+        <v>0.8055555555555555</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="K51" t="n">

</xml_diff>